<commit_message>
Drosophila Drift Experiment Done
</commit_message>
<xml_diff>
--- a/Semester_3/Biology_Practicals/Observations/Final_Data.xlsx
+++ b/Semester_3/Biology_Practicals/Observations/Final_Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8820"/>
   </bookViews>
   <sheets>
     <sheet name="Final DARK" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Generation1 (Light)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="540" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="36">
   <si>
     <t>G1</t>
   </si>
@@ -126,6 +127,15 @@
   </si>
   <si>
     <t>G1*</t>
+  </si>
+  <si>
+    <t>Mating Success of White Males</t>
+  </si>
+  <si>
+    <t>Egg to Adult Survivorship (Red)</t>
+  </si>
+  <si>
+    <t>Egg to Adult Survivorship (White)</t>
   </si>
 </sst>
 </file>
@@ -483,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M64"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N61" sqref="N61"/>
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,6 +1882,33 @@
         <v>0.14480139626426586</v>
       </c>
     </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>33</v>
+      </c>
+      <c r="E66">
+        <f>I60/0.5</f>
+        <v>0.4781932602119765</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68">
+        <f>F59/0.5</f>
+        <v>1.2730765403958175</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>35</v>
+      </c>
+      <c r="E69">
+        <f>F60/0.5</f>
+        <v>0.72692345960418259</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1879,10 +1916,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M64"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66:E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3266,6 +3303,33 @@
       <c r="M64" s="2">
         <f>_xlfn.STDEV.S(L12,L25,L38,L51)</f>
         <v>0.1076924878651556</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>33</v>
+      </c>
+      <c r="E66">
+        <f>I60/0.5</f>
+        <v>0.60184056374178585</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68">
+        <f>F59/0.5</f>
+        <v>1.0757681956750873</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>35</v>
+      </c>
+      <c r="E69">
+        <f>F60/0.5</f>
+        <v>0.92423180432491281</v>
       </c>
     </row>
   </sheetData>
@@ -3278,7 +3342,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:H8"/>
     </sheetView>
   </sheetViews>
@@ -3651,7 +3715,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>

</xml_diff>